<commit_message>
Fix unit display logic in Excel invoice export
</commit_message>
<xml_diff>
--- a/api/components/請求書テンプレート.xlsx
+++ b/api/components/請求書テンプレート.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\almeida.ped_redhorse\Documents\GitHub\rht-hotel\api\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433CA619-BC07-4807-B479-AFAE527AA0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35216BC-1C34-495A-82FB-94A2514D0F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23475" yWindow="6195" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-1670" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="請求書フォーマット" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,7 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="178" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -738,98 +738,32 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="6" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -857,18 +791,84 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1131,7 +1131,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:O2"/>
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1155,25 +1155,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="3"/>
@@ -1183,19 +1183,19 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="20"/>
+      <c r="K2" s="43"/>
       <c r="L2" s="70" t="e">
         <f>EDATE(D10+1,-1)-1</f>
         <v>#NUM!</v>
@@ -1236,14 +1236,14 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
       <c r="I4" s="5"/>
       <c r="J4" s="3" t="s">
         <v>3</v>
@@ -1261,16 +1261,16 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1311,16 +1311,16 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1361,28 +1361,28 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="33" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="3"/>
       <c r="S9" s="7"/>
@@ -1395,26 +1395,26 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="69"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="52" t="s">
+      <c r="J10" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="3"/>
       <c r="S10" s="10"/>
@@ -1427,24 +1427,24 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="31"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="27"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="53"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="3"/>
       <c r="S11" s="10"/>
@@ -1457,22 +1457,22 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="39"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="29"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="57"/>
       <c r="Q12" s="9"/>
       <c r="R12" s="3"/>
       <c r="S12" s="7"/>
@@ -1485,22 +1485,22 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="39"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="53"/>
-      <c r="P13" s="53"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="3"/>
       <c r="S13" s="7"/>
@@ -1513,24 +1513,24 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="42"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="24"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
@@ -1552,15 +1552,15 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="34" t="s">
+      <c r="J15" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
@@ -1573,22 +1573,22 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="47">
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="49">
         <f>I24</f>
         <v>0</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="48" t="s">
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="20"/>
+      <c r="I16" s="43"/>
       <c r="J16" s="12"/>
       <c r="K16" s="3"/>
       <c r="L16" s="9"/>
@@ -1608,15 +1608,15 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="12"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1667,27 +1667,27 @@
       <c r="A19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="32" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="29"/>
-      <c r="I19" s="54" t="s">
+      <c r="H19" s="21"/>
+      <c r="I19" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="29"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="21"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
@@ -1704,25 +1704,25 @@
         <f>_xlfn.IFS(B20&gt;0,1,B20="","")</f>
         <v>1</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="49"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="29"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="21"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
@@ -1736,21 +1736,21 @@
     </row>
     <row r="21" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="29"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="21"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
@@ -1764,21 +1764,21 @@
     </row>
     <row r="22" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="6"/>
       <c r="H22" s="15"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="21"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
@@ -1792,21 +1792,21 @@
     </row>
     <row r="23" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="29"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="21"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
@@ -1825,21 +1825,21 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="66" t="s">
+      <c r="G24" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="29"/>
-      <c r="I24" s="50">
+      <c r="H24" s="21"/>
+      <c r="I24" s="46">
         <f>SUM(I20:K23)</f>
         <v>0</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="29"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="21"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -1857,21 +1857,21 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="55" t="s">
+      <c r="G25" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="51">
+      <c r="H25" s="24"/>
+      <c r="I25" s="31">
         <f>ROUNDDOWN(I24*0.1/1.1,0)</f>
         <v>0</v>
       </c>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="42"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="24"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
@@ -1919,21 +1919,21 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="56" t="s">
+      <c r="G27" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="42"/>
-      <c r="I27" s="51">
+      <c r="H27" s="24"/>
+      <c r="I27" s="31">
         <f>I24-ROUNDDOWN(I24*0.1/1.1,0)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="42"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="24"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
@@ -1952,21 +1952,21 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="55" t="s">
+      <c r="G28" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="42"/>
-      <c r="I28" s="51">
+      <c r="H28" s="24"/>
+      <c r="I28" s="31">
         <f>ROUNDDOWN(I24*0.1/1.1,0)</f>
         <v>0</v>
       </c>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="42"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="24"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
@@ -2013,18 +2013,18 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="56" t="s">
+      <c r="G30" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H30" s="42"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="42"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="24"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
@@ -2043,18 +2043,18 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="55" t="s">
+      <c r="G31" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
-      <c r="M31" s="41"/>
-      <c r="N31" s="41"/>
-      <c r="O31" s="41"/>
-      <c r="P31" s="42"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="24"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
@@ -2095,26 +2095,26 @@
       <c r="Z32" s="3"/>
     </row>
     <row r="33" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="57" t="s">
+      <c r="B33" s="27"/>
+      <c r="C33" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="59"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34"/>
+      <c r="P33" s="35"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
@@ -2127,22 +2127,22 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="61"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="61"/>
-      <c r="P34" s="62"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="37"/>
+      <c r="O34" s="37"/>
+      <c r="P34" s="38"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
@@ -2155,22 +2155,22 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="61"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="61"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="61"/>
-      <c r="P35" s="62"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="37"/>
+      <c r="P35" s="38"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
@@ -2183,24 +2183,24 @@
       <c r="Z35" s="3"/>
     </row>
     <row r="36" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A36" s="40"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="63" t="s">
+      <c r="A36" s="30"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="K36" s="64"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="64"/>
-      <c r="N36" s="64"/>
-      <c r="O36" s="64"/>
-      <c r="P36" s="65"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="41"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
@@ -29038,19 +29038,32 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A33:B36"/>
-    <mergeCell ref="I31:P31"/>
-    <mergeCell ref="I28:P28"/>
-    <mergeCell ref="I30:P30"/>
-    <mergeCell ref="C33:P35"/>
-    <mergeCell ref="C36:P36"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="J9:P9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C14"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="J14:P14"/>
+    <mergeCell ref="J10:P13"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="D16:G17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="J15:P15"/>
     <mergeCell ref="I19:P19"/>
     <mergeCell ref="I20:P20"/>
@@ -29063,40 +29076,24 @@
     <mergeCell ref="I24:P24"/>
     <mergeCell ref="I25:P25"/>
     <mergeCell ref="I27:P27"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="D16:G17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J9:P9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C14"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="J14:P14"/>
-    <mergeCell ref="J10:P13"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A33:B36"/>
+    <mergeCell ref="I31:P31"/>
+    <mergeCell ref="I28:P28"/>
+    <mergeCell ref="I30:P30"/>
+    <mergeCell ref="C33:P35"/>
+    <mergeCell ref="C36:P36"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="G24:H24"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20:H23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"個,泊,名,日,ヶ月"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H21:H23" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>$R$9:$R$13</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Revert "Merge pull request #151 from almeida-rht/refactor/billing-page"
This reverts commit d66aea245fdfd172ce4192f4769f81b4c54af6c5, reversing
changes made to b812c5f6764031d06c6d4396fad75ebd044a6f6a.
</commit_message>
<xml_diff>
--- a/api/components/請求書テンプレート.xlsx
+++ b/api/components/請求書テンプレート.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\almeida.ped_redhorse\Documents\GitHub\rht-hotel\api\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35216BC-1C34-495A-82FB-94A2514D0F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433CA619-BC07-4807-B479-AFAE527AA0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-1670" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23475" yWindow="6195" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="請求書フォーマット" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,7 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="178" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -738,32 +738,98 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="6" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -791,84 +857,18 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1131,7 +1131,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+      <selection activeCell="L2" sqref="L2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1155,25 +1155,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="43"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="3"/>
@@ -1183,19 +1183,19 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="67" t="s">
+      <c r="J2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="43"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="70" t="e">
         <f>EDATE(D10+1,-1)-1</f>
         <v>#NUM!</v>
@@ -1236,14 +1236,14 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="5"/>
       <c r="J4" s="3" t="s">
         <v>3</v>
@@ -1261,16 +1261,16 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1311,16 +1311,16 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1361,28 +1361,28 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="19" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="52" t="s">
+      <c r="J9" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="3"/>
       <c r="S9" s="7"/>
@@ -1395,26 +1395,26 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="69"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
-      <c r="P10" s="57"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="53"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="3"/>
       <c r="S10" s="10"/>
@@ -1427,24 +1427,24 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="31"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="3"/>
       <c r="S11" s="10"/>
@@ -1457,22 +1457,22 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="29"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="39"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57"/>
-      <c r="P12" s="57"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
       <c r="Q12" s="9"/>
       <c r="R12" s="3"/>
       <c r="S12" s="7"/>
@@ -1485,22 +1485,22 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="29"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="57"/>
-      <c r="P13" s="57"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="53"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="3"/>
       <c r="S13" s="7"/>
@@ -1513,24 +1513,24 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="24"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="42"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="42" t="s">
+      <c r="J14" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
@@ -1552,15 +1552,15 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="42" t="s">
+      <c r="J15" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
@@ -1573,22 +1573,22 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="49">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="47">
         <f>I24</f>
         <v>0</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="50" t="s">
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="43"/>
+      <c r="I16" s="20"/>
       <c r="J16" s="12"/>
       <c r="K16" s="3"/>
       <c r="L16" s="9"/>
@@ -1608,15 +1608,15 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="12"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1667,27 +1667,27 @@
       <c r="A19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="51" t="s">
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="44" t="s">
+      <c r="H19" s="29"/>
+      <c r="I19" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="21"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="29"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
@@ -1704,25 +1704,25 @@
         <f>_xlfn.IFS(B20&gt;0,1,B20="","")</f>
         <v>1</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="45"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="21"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="29"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
@@ -1736,21 +1736,21 @@
     </row>
     <row r="21" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="21"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="29"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
@@ -1764,21 +1764,21 @@
     </row>
     <row r="22" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
       <c r="G22" s="6"/>
       <c r="H22" s="15"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="21"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="29"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
@@ -1792,21 +1792,21 @@
     </row>
     <row r="23" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="21"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="29"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
@@ -1825,21 +1825,21 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="46">
+      <c r="H24" s="29"/>
+      <c r="I24" s="50">
         <f>SUM(I20:K23)</f>
         <v>0</v>
       </c>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="21"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="29"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -1857,21 +1857,21 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="25" t="s">
+      <c r="G25" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="24"/>
-      <c r="I25" s="31">
+      <c r="H25" s="42"/>
+      <c r="I25" s="51">
         <f>ROUNDDOWN(I24*0.1/1.1,0)</f>
         <v>0</v>
       </c>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="24"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="42"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
@@ -1919,21 +1919,21 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="24"/>
-      <c r="I27" s="31">
+      <c r="H27" s="42"/>
+      <c r="I27" s="51">
         <f>I24-ROUNDDOWN(I24*0.1/1.1,0)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="32"/>
-      <c r="O27" s="32"/>
-      <c r="P27" s="24"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="42"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
@@ -1952,21 +1952,21 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="25" t="s">
+      <c r="G28" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="24"/>
-      <c r="I28" s="31">
+      <c r="H28" s="42"/>
+      <c r="I28" s="51">
         <f>ROUNDDOWN(I24*0.1/1.1,0)</f>
         <v>0</v>
       </c>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="32"/>
-      <c r="O28" s="32"/>
-      <c r="P28" s="24"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="42"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
@@ -2013,18 +2013,18 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="H30" s="24"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="24"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="42"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
@@ -2043,18 +2043,18 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="25" t="s">
+      <c r="G31" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="24"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="24"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="42"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
@@ -2095,26 +2095,26 @@
       <c r="Z32" s="3"/>
     </row>
     <row r="33" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="33" t="s">
+      <c r="B33" s="31"/>
+      <c r="C33" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="34"/>
-      <c r="P33" s="35"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="59"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
@@ -2127,22 +2127,22 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="38"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="61"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="61"/>
+      <c r="P34" s="62"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
@@ -2155,22 +2155,22 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="37"/>
-      <c r="P35" s="38"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="61"/>
+      <c r="L35" s="61"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="61"/>
+      <c r="O35" s="61"/>
+      <c r="P35" s="62"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
@@ -2183,24 +2183,24 @@
       <c r="Z35" s="3"/>
     </row>
     <row r="36" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A36" s="30"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="39" t="s">
+      <c r="A36" s="40"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="40"/>
-      <c r="O36" s="40"/>
-      <c r="P36" s="41"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="64"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="64"/>
+      <c r="N36" s="64"/>
+      <c r="O36" s="64"/>
+      <c r="P36" s="65"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
@@ -29038,32 +29038,19 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="J9:P9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C14"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="J14:P14"/>
-    <mergeCell ref="J10:P13"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="D16:G17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A33:B36"/>
+    <mergeCell ref="I31:P31"/>
+    <mergeCell ref="I28:P28"/>
+    <mergeCell ref="I30:P30"/>
+    <mergeCell ref="C33:P35"/>
+    <mergeCell ref="C36:P36"/>
     <mergeCell ref="J15:P15"/>
     <mergeCell ref="I19:P19"/>
     <mergeCell ref="I20:P20"/>
@@ -29076,24 +29063,40 @@
     <mergeCell ref="I24:P24"/>
     <mergeCell ref="I25:P25"/>
     <mergeCell ref="I27:P27"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A33:B36"/>
-    <mergeCell ref="I31:P31"/>
-    <mergeCell ref="I28:P28"/>
-    <mergeCell ref="I30:P30"/>
-    <mergeCell ref="C33:P35"/>
-    <mergeCell ref="C36:P36"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="D16:G17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J9:P9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C14"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="J14:P14"/>
+    <mergeCell ref="J10:P13"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:O2"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20:H23" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"個,泊,名,日,ヶ月"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H21:H23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>$R$9:$R$13</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
refactor(billing): overhaul invoice generation and billing list with detailed tax breakdowns and feature-based frontend structure
</commit_message>
<xml_diff>
--- a/api/components/請求書テンプレート.xlsx
+++ b/api/components/請求書テンプレート.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\almeida.ped_redhorse\Documents\GitHub\rht-hotel\api\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433CA619-BC07-4807-B479-AFAE527AA0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35216BC-1C34-495A-82FB-94A2514D0F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23475" yWindow="6195" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-1670" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="請求書フォーマット" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,7 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="178" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -738,98 +738,32 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="6" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -857,18 +791,84 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1131,7 +1131,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:O2"/>
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1155,25 +1155,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="3"/>
@@ -1183,19 +1183,19 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="20"/>
+      <c r="K2" s="43"/>
       <c r="L2" s="70" t="e">
         <f>EDATE(D10+1,-1)-1</f>
         <v>#NUM!</v>
@@ -1236,14 +1236,14 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
       <c r="I4" s="5"/>
       <c r="J4" s="3" t="s">
         <v>3</v>
@@ -1261,16 +1261,16 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1311,16 +1311,16 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1361,28 +1361,28 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="33" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="3"/>
       <c r="S9" s="7"/>
@@ -1395,26 +1395,26 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="69"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="52" t="s">
+      <c r="J10" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="3"/>
       <c r="S10" s="10"/>
@@ -1427,24 +1427,24 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="31"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="27"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="53"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="3"/>
       <c r="S11" s="10"/>
@@ -1457,22 +1457,22 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="39"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="29"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="57"/>
       <c r="Q12" s="9"/>
       <c r="R12" s="3"/>
       <c r="S12" s="7"/>
@@ -1485,22 +1485,22 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="39"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="53"/>
-      <c r="P13" s="53"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="3"/>
       <c r="S13" s="7"/>
@@ -1513,24 +1513,24 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="42"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="24"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
@@ -1552,15 +1552,15 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="34" t="s">
+      <c r="J15" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
@@ -1573,22 +1573,22 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="47">
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="49">
         <f>I24</f>
         <v>0</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="48" t="s">
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="20"/>
+      <c r="I16" s="43"/>
       <c r="J16" s="12"/>
       <c r="K16" s="3"/>
       <c r="L16" s="9"/>
@@ -1608,15 +1608,15 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="12"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1667,27 +1667,27 @@
       <c r="A19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="32" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="29"/>
-      <c r="I19" s="54" t="s">
+      <c r="H19" s="21"/>
+      <c r="I19" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="29"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="21"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
@@ -1704,25 +1704,25 @@
         <f>_xlfn.IFS(B20&gt;0,1,B20="","")</f>
         <v>1</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="49"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="29"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="21"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
@@ -1736,21 +1736,21 @@
     </row>
     <row r="21" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="29"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="21"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
@@ -1764,21 +1764,21 @@
     </row>
     <row r="22" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="6"/>
       <c r="H22" s="15"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="21"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
@@ -1792,21 +1792,21 @@
     </row>
     <row r="23" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="29"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="21"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
@@ -1825,21 +1825,21 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="66" t="s">
+      <c r="G24" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="29"/>
-      <c r="I24" s="50">
+      <c r="H24" s="21"/>
+      <c r="I24" s="46">
         <f>SUM(I20:K23)</f>
         <v>0</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="29"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="21"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -1857,21 +1857,21 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="55" t="s">
+      <c r="G25" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="51">
+      <c r="H25" s="24"/>
+      <c r="I25" s="31">
         <f>ROUNDDOWN(I24*0.1/1.1,0)</f>
         <v>0</v>
       </c>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="42"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="24"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
@@ -1919,21 +1919,21 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="56" t="s">
+      <c r="G27" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="42"/>
-      <c r="I27" s="51">
+      <c r="H27" s="24"/>
+      <c r="I27" s="31">
         <f>I24-ROUNDDOWN(I24*0.1/1.1,0)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="42"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="24"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
@@ -1952,21 +1952,21 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="55" t="s">
+      <c r="G28" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="42"/>
-      <c r="I28" s="51">
+      <c r="H28" s="24"/>
+      <c r="I28" s="31">
         <f>ROUNDDOWN(I24*0.1/1.1,0)</f>
         <v>0</v>
       </c>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="42"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="24"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
@@ -2013,18 +2013,18 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="56" t="s">
+      <c r="G30" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H30" s="42"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="42"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="24"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
@@ -2043,18 +2043,18 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="55" t="s">
+      <c r="G31" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
-      <c r="M31" s="41"/>
-      <c r="N31" s="41"/>
-      <c r="O31" s="41"/>
-      <c r="P31" s="42"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="24"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
@@ -2095,26 +2095,26 @@
       <c r="Z32" s="3"/>
     </row>
     <row r="33" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="57" t="s">
+      <c r="B33" s="27"/>
+      <c r="C33" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="59"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34"/>
+      <c r="P33" s="35"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
@@ -2127,22 +2127,22 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="61"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="61"/>
-      <c r="P34" s="62"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="37"/>
+      <c r="O34" s="37"/>
+      <c r="P34" s="38"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
@@ -2155,22 +2155,22 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="61"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="61"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="61"/>
-      <c r="P35" s="62"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="37"/>
+      <c r="P35" s="38"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
@@ -2183,24 +2183,24 @@
       <c r="Z35" s="3"/>
     </row>
     <row r="36" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A36" s="40"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="63" t="s">
+      <c r="A36" s="30"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="K36" s="64"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="64"/>
-      <c r="N36" s="64"/>
-      <c r="O36" s="64"/>
-      <c r="P36" s="65"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="41"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
@@ -29038,19 +29038,32 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A33:B36"/>
-    <mergeCell ref="I31:P31"/>
-    <mergeCell ref="I28:P28"/>
-    <mergeCell ref="I30:P30"/>
-    <mergeCell ref="C33:P35"/>
-    <mergeCell ref="C36:P36"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="J9:P9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C14"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="J14:P14"/>
+    <mergeCell ref="J10:P13"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="D16:G17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="J15:P15"/>
     <mergeCell ref="I19:P19"/>
     <mergeCell ref="I20:P20"/>
@@ -29063,40 +29076,24 @@
     <mergeCell ref="I24:P24"/>
     <mergeCell ref="I25:P25"/>
     <mergeCell ref="I27:P27"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="D16:G17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J9:P9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C14"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="J14:P14"/>
-    <mergeCell ref="J10:P13"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A33:B36"/>
+    <mergeCell ref="I31:P31"/>
+    <mergeCell ref="I28:P28"/>
+    <mergeCell ref="I30:P30"/>
+    <mergeCell ref="C33:P35"/>
+    <mergeCell ref="C36:P36"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="G24:H24"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20:H23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"個,泊,名,日,ヶ月"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H21:H23" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>$R$9:$R$13</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>

</xml_diff>